<commit_message>
added root node for Babylon
</commit_message>
<xml_diff>
--- a/axisSummary.xlsx
+++ b/axisSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cloudadmincombeenation.sharepoint.com/sites/CbnAzureAD/Shared Documents/General/3D/Library/debugAxis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61C1172D-C2F5-4311-82E1-941D10A16F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{61C1172D-C2F5-4311-82E1-941D10A16F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E2A3EFA-F097-452A-9B0D-E315FC28E251}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2595" windowWidth="29040" windowHeight="16440" xr2:uid="{BC2362F8-06B1-4DB4-82F8-555C43C3FB55}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
   <si>
     <t>Source</t>
   </si>
@@ -117,6 +117,36 @@
   </si>
   <si>
     <t>debugAxisGLBtoBabylonRH.babylon</t>
+  </si>
+  <si>
+    <t>Import converted Scene CS</t>
+  </si>
+  <si>
+    <t>https://playground.babylonjs.com/#VSIJLQ#4</t>
+  </si>
+  <si>
+    <t>MIRRORED</t>
+  </si>
+  <si>
+    <t>https://playground.babylonjs.com/#VSIJLQ#5</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>The scaling and rotation is not removed automatically from __root__ anymore. When manually removed, it is correct again and works like ID2</t>
+  </si>
+  <si>
+    <t>https://playground.babylonjs.com/#VSIJLQ#6</t>
+  </si>
+  <si>
+    <t>The scaling and rotation is not applied automatically to __root__ anymore. When manually added, it is correct again and works like ID1</t>
+  </si>
+  <si>
+    <t>https://playground.babylonjs.com/#VSIJLQ#7</t>
   </si>
 </sst>
 </file>
@@ -152,8 +182,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -468,171 +501,610 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2384E4E-9A47-46B1-A2CF-C3CAFFA094B9}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1"/>
-    <col min="9" max="9" width="43.7109375" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="7" width="33.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" customWidth="1"/>
+    <col min="11" max="11" width="43.7109375" customWidth="1"/>
+    <col min="12" max="12" width="24.85546875" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" customWidth="1"/>
+    <col min="14" max="14" width="31.85546875" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" customWidth="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>25</v>
       </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
         <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E72EB2B3AE284544862E6B8F424A3082" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="dce2b5844722693021f6851ad5839323">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="03c733eb-657e-42a3-b6c2-09a394e9851c" xmlns:ns3="b54ac89a-b092-4fa0-8518-e21dc3e7c43c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="174dbdd30788cebd8d5aa5bca5d56fba" ns2:_="" ns3:_="">
+    <xsd:import namespace="03c733eb-657e-42a3-b6c2-09a394e9851c"/>
+    <xsd:import namespace="b54ac89a-b092-4fa0-8518-e21dc3e7c43c"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="03c733eb-657e-42a3-b6c2-09a394e9851c" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="11" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="12" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="15" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildmarkierungen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="89d124c7-a5ab-4fc2-b3ef-10e5e26ceccb" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b54ac89a-b092-4fa0-8518-e21dc3e7c43c" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Freigegeben für" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Freigegeben für - Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{84245507-2256-4673-a880-285cef59ee4f}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="b54ac89a-b092-4fa0-8518-e21dc3e7c43c">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="03c733eb-657e-42a3-b6c2-09a394e9851c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b54ac89a-b092-4fa0-8518-e21dc3e7c43c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D88931AD-A739-48FC-87C1-70C53AAFEF2B}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17EE1BC2-FC05-460F-9DFB-9374DCF663A3}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F7C8773-4597-43FE-8D38-6A61788B3376}"/>
 </file>
</xml_diff>